<commit_message>
Facebook Integration Module Requirements
</commit_message>
<xml_diff>
--- a/FacebookIntegration/Documents/FaceBookComponent.xlsx
+++ b/FacebookIntegration/Documents/FaceBookComponent.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="14355" windowHeight="4680" activeTab="2"/>
@@ -316,7 +316,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
@@ -324,7 +324,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -740,6 +740,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -752,9 +755,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="26">
@@ -870,7 +870,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -905,7 +904,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1081,47 +1079,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="59" t="s">
+    <row r="4" spans="1:7">
+      <c r="A4" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-    </row>
-    <row r="5" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="60" t="s">
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+    </row>
+    <row r="5" spans="1:7" ht="24.75" customHeight="1">
+      <c r="A5" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="61" t="s">
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="61"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="61"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1135,14 +1133,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="3" width="30.28515625" style="4" customWidth="1"/>
     <col min="4" max="4" width="20.5703125" style="4" customWidth="1"/>
@@ -1152,7 +1150,7 @@
     <col min="8" max="8" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1162,7 +1160,7 @@
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.75">
       <c r="A2" s="6" t="s">
         <v>8</v>
       </c>
@@ -1186,7 +1184,7 @@
       </c>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="29" t="s">
         <v>12</v>
       </c>
@@ -1210,7 +1208,7 @@
       </c>
       <c r="H3" s="11"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="8" t="s">
         <v>13</v>
       </c>
@@ -1234,7 +1232,7 @@
       </c>
       <c r="H4" s="11"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="12" t="s">
         <v>21</v>
       </c>
@@ -1258,7 +1256,7 @@
       </c>
       <c r="H5" s="11"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="29" t="s">
         <v>14</v>
       </c>
@@ -1282,7 +1280,7 @@
       </c>
       <c r="H6" s="23"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="8" t="s">
         <v>15</v>
       </c>
@@ -1313,17 +1311,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="25.7109375" style="4" bestFit="1" customWidth="1"/>
@@ -1332,7 +1330,7 @@
     <col min="5" max="5" width="37.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="31.5">
       <c r="A1" s="43" t="s">
         <v>2</v>
       </c>
@@ -1352,7 +1350,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="51" customFormat="1">
       <c r="A2" s="49">
         <v>1</v>
       </c>
@@ -1365,7 +1363,7 @@
       <c r="D2" s="49"/>
       <c r="E2" s="50"/>
     </row>
-    <row r="3" spans="1:7" s="51" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="51" customFormat="1" ht="30">
       <c r="A3" s="49">
         <v>2</v>
       </c>
@@ -1378,7 +1376,7 @@
       <c r="D3" s="49"/>
       <c r="E3" s="50"/>
     </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="45">
       <c r="A4" s="41">
         <v>3</v>
       </c>
@@ -1396,7 +1394,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="35">
         <v>4</v>
       </c>
@@ -1414,7 +1412,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="47" customFormat="1">
       <c r="A6" s="53">
         <v>5</v>
       </c>
@@ -1425,7 +1423,7 @@
       <c r="D6" s="54"/>
       <c r="E6" s="54"/>
     </row>
-    <row r="7" spans="1:7" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="51" customFormat="1">
       <c r="A7" s="48">
         <v>6</v>
       </c>
@@ -1438,7 +1436,7 @@
       <c r="D7" s="50"/>
       <c r="E7" s="50"/>
     </row>
-    <row r="8" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="135">
       <c r="A8" s="35">
         <v>7</v>
       </c>
@@ -1458,7 +1456,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="30">
       <c r="A9" s="45">
         <v>8</v>
       </c>
@@ -1481,7 +1479,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="30">
       <c r="A10" s="41">
         <v>9</v>
       </c>
@@ -1500,11 +1498,11 @@
       <c r="F10" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="G10" s="64" t="s">
+      <c r="G10" s="59" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="30">
       <c r="A11" s="53">
         <v>10</v>
       </c>
@@ -1524,7 +1522,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="45">
       <c r="A12" s="53">
         <v>11</v>
       </c>
@@ -1542,7 +1540,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="30">
       <c r="A13" s="41">
         <v>12</v>
       </c>
@@ -1559,7 +1557,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="30">
       <c r="A14" s="35">
         <v>13</v>
       </c>
@@ -1574,7 +1572,7 @@
       </c>
       <c r="E14" s="42"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="45"/>
       <c r="B15" s="46"/>
       <c r="C15" s="46"/>
@@ -1586,7 +1584,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="30">
       <c r="A16" s="57">
         <v>15</v>
       </c>
@@ -1603,7 +1601,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="30">
       <c r="A17" s="53">
         <v>16</v>
       </c>
@@ -1620,7 +1618,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1628,7 +1626,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1639,7 +1637,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1647,7 +1645,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="58">
         <v>20</v>
       </c>
@@ -1664,20 +1662,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="95.5703125" customWidth="1"/>
     <col min="3" max="3" width="56.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="16" t="s">
         <v>2</v>
       </c>
@@ -1688,154 +1686,154 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="18">
         <v>1</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="19"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="18">
         <v>2</v>
       </c>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="36">
         <v>3</v>
       </c>
       <c r="B4" s="17"/>
       <c r="C4" s="17"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="36">
         <v>4</v>
       </c>
       <c r="B5" s="35"/>
       <c r="C5" s="35"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="36">
         <v>6</v>
       </c>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="36">
         <v>7</v>
       </c>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="36">
         <v>8</v>
       </c>
       <c r="B8" s="42"/>
       <c r="C8" s="40"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="36">
         <v>9</v>
       </c>
       <c r="B9" s="42"/>
       <c r="C9" s="40"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="36">
         <v>10</v>
       </c>
       <c r="B10" s="42"/>
       <c r="C10" s="40"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="36">
         <v>11</v>
       </c>
       <c r="B11" s="42"/>
       <c r="C11" s="40"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="36">
         <v>12</v>
       </c>
       <c r="B12" s="42"/>
       <c r="C12" s="40"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="36">
         <v>13</v>
       </c>
       <c r="B13" s="42"/>
       <c r="C13" s="40"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="36">
         <v>14</v>
       </c>
       <c r="B14" s="42"/>
       <c r="C14" s="40"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="36">
         <v>15</v>
       </c>
       <c r="B15" s="42"/>
       <c r="C15" s="40"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="36">
         <v>16</v>
       </c>
       <c r="B16" s="42"/>
       <c r="C16" s="40"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="36">
         <v>17</v>
       </c>
       <c r="B17" s="42"/>
       <c r="C17" s="40"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="36">
         <v>18</v>
       </c>
       <c r="B18" s="42"/>
       <c r="C18" s="40"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" s="36">
         <v>19</v>
       </c>
       <c r="B19" s="42"/>
       <c r="C19" s="40"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="36">
         <v>20</v>
       </c>
       <c r="B20" s="42"/>
       <c r="C20" s="40"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="36">
         <v>21</v>
       </c>
       <c r="B21" s="42"/>
       <c r="C21" s="40"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3">
       <c r="A22" s="36">
         <v>22</v>
       </c>
       <c r="B22" s="42"/>
       <c r="C22" s="40"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" s="36">
         <v>23</v>
       </c>
@@ -1848,20 +1846,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" customWidth="1"/>
     <col min="2" max="2" width="83.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75">
       <c r="A1" s="14" t="s">
         <v>2</v>
       </c>
@@ -1869,7 +1867,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="44">
         <v>1</v>
       </c>
@@ -1877,23 +1875,23 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="30">
         <v>2</v>
       </c>
       <c r="B3" s="30"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="44">
         <v>3</v>
       </c>
       <c r="B4" s="44"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="44"/>
       <c r="B5" s="44"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="30"/>
       <c r="B6" s="30"/>
     </row>
@@ -1903,31 +1901,31 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="47.5703125" customWidth="1"/>
     <col min="5" max="5" width="66.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="63"/>
+      <c r="B1" s="64"/>
       <c r="C1" s="24"/>
-      <c r="D1" s="62" t="s">
+      <c r="D1" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="63"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E1" s="64"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75">
       <c r="A2" s="20" t="s">
         <v>2</v>
       </c>
@@ -1942,7 +1940,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="25">
         <v>1</v>
       </c>
@@ -1957,7 +1955,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="25">
         <v>2</v>
       </c>
@@ -1970,7 +1968,7 @@
       </c>
       <c r="E4" s="15"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="25">
         <v>3</v>
       </c>
@@ -1983,7 +1981,7 @@
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="25">
         <v>4</v>
       </c>
@@ -1996,7 +1994,7 @@
       </c>
       <c r="E6" s="15"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="25">
         <v>5</v>
       </c>
@@ -2007,7 +2005,7 @@
       </c>
       <c r="E7" s="15"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="25">
         <v>6</v>
       </c>
@@ -2018,7 +2016,7 @@
       </c>
       <c r="E8" s="15"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="25">
         <v>7</v>
       </c>
@@ -2029,7 +2027,7 @@
       </c>
       <c r="E9" s="13"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="25">
         <v>8</v>
       </c>
@@ -2040,7 +2038,7 @@
       </c>
       <c r="E10" s="15"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="25"/>
       <c r="B11" s="28"/>
       <c r="C11" s="27"/>
@@ -2049,7 +2047,7 @@
       </c>
       <c r="E11" s="15"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="25"/>
       <c r="B12" s="28"/>
       <c r="C12" s="27"/>
@@ -2058,7 +2056,7 @@
       </c>
       <c r="E12" s="15"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="25"/>
       <c r="B13" s="28"/>
       <c r="C13" s="27"/>
@@ -2077,21 +2075,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="11.42578125" customWidth="1"/>
     <col min="3" max="3" width="29.28515625" customWidth="1"/>
     <col min="4" max="4" width="59.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75">
       <c r="A1" s="31" t="s">
         <v>2</v>
       </c>
@@ -2103,7 +2101,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="60">
       <c r="A2" s="33">
         <v>1</v>
       </c>
@@ -2117,7 +2115,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="30">
       <c r="A3" s="33">
         <v>2</v>
       </c>
@@ -2127,7 +2125,7 @@
       </c>
       <c r="D3" s="32"/>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="30">
       <c r="A4" s="33">
         <v>3</v>
       </c>
@@ -2137,7 +2135,7 @@
       </c>
       <c r="D4" s="32"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="33">
         <v>4</v>
       </c>
@@ -2147,7 +2145,7 @@
       </c>
       <c r="D5" s="32"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="33">
         <v>5</v>
       </c>
@@ -2157,7 +2155,7 @@
       </c>
       <c r="D6" s="32"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="33">
         <v>6</v>
       </c>
@@ -2167,7 +2165,7 @@
       </c>
       <c r="D7" s="32"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="33">
         <v>7</v>
       </c>
@@ -2175,7 +2173,7 @@
       <c r="C8" s="32"/>
       <c r="D8" s="32"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="33">
         <v>8</v>
       </c>
@@ -2183,7 +2181,7 @@
       <c r="C9" s="32"/>
       <c r="D9" s="32"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="33">
         <v>9</v>
       </c>
@@ -2191,7 +2189,7 @@
       <c r="C10" s="32"/>
       <c r="D10" s="32"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="33">
         <v>10</v>
       </c>

</xml_diff>